<commit_message>
Fixed the iteration process
Yup
</commit_message>
<xml_diff>
--- a/RPSD Propellant Info.xlsx
+++ b/RPSD Propellant Info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nevermore\Documents\IVDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nevermore\Documents\GitHub\Spacecraft-Propulsion-System-Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>RPSD Propellant Information Sheet</t>
   </si>
@@ -59,16 +59,16 @@
     <t>Cp [kJ/kgK]</t>
   </si>
   <si>
-    <t>Cv [kJ/kgK]</t>
-  </si>
-  <si>
     <t>Molar Mass [kg/mol]</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Freon [R-22]</t>
+  </si>
+  <si>
+    <t>Carbon Dioxide</t>
+  </si>
+  <si>
+    <t>Cp [J/kgK]</t>
   </si>
 </sst>
 </file>
@@ -76,7 +76,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="175" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -101,7 +101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -152,11 +152,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -167,25 +178,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -408,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -420,173 +443,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>2.016E-3</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>1.67</v>
       </c>
       <c r="E3" s="2">
         <v>14.32</v>
       </c>
       <c r="F3" s="2">
-        <v>10.16</v>
+        <f>E3*1000</f>
+        <v>14320</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>4.0026020000000001E-3</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1.67</v>
       </c>
       <c r="E4" s="1">
         <v>14.32</v>
       </c>
-      <c r="F4" s="1">
-        <v>10.16</v>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F9" si="0">E4*1000</f>
+        <v>14320</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>2.8013400000000001E-2</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>1.4</v>
       </c>
       <c r="E5" s="1">
         <v>1.04</v>
       </c>
-      <c r="F5" s="1">
-        <v>0.74299999999999999</v>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>1040</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="7">
         <v>8.6480000000000001E-2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>1.18</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>2.0178999999999999E-2</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>1.67</v>
       </c>
       <c r="E7" s="1">
         <v>1.03</v>
       </c>
-      <c r="F7" s="1">
-        <v>0.61799999999999999</v>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>1030</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>0.1313</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>1.67</v>
       </c>
       <c r="E8" s="1">
         <v>0.16</v>
       </c>
-      <c r="F8" s="1">
-        <v>9.7000000000000003E-2</v>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>3.9947999999999997E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>1.67</v>
       </c>
       <c r="E9" s="1">
         <v>0.52</v>
       </c>
-      <c r="F9" s="1">
-        <v>0.312</v>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="12">
+        <v>4.4010000000000001E-2</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>